<commit_message>
Added better display in descriptors.py; fixed some bugs
</commit_message>
<xml_diff>
--- a/data/descriptor builder.xlsx
+++ b/data/descriptor builder.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -56,13 +56,13 @@
     <t>Secondary</t>
   </si>
   <si>
+    <t>Contact Only</t>
+  </si>
+  <si>
     <t>slugging</t>
   </si>
   <si>
     <t>smallball</t>
-  </si>
-  <si>
-    <t>fancy</t>
   </si>
   <si>
     <t>Weak Slugger</t>
@@ -92,9 +92,6 @@
     <t>fancy: control, sparkle, strategy</t>
   </si>
   <si>
-    <t>smallball: contact, control, speed</t>
-  </si>
-  <si>
     <t>manufacture: speed, bravery, timing, discipline</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Weak Baserunner</t>
   </si>
   <si>
-    <t>Weak Strategy Hitter</t>
-  </si>
-  <si>
     <t>Versatile Hitter</t>
   </si>
   <si>
@@ -114,6 +108,27 @@
   </si>
   <si>
     <t>Slow Hitter</t>
+  </si>
+  <si>
+    <t>smallball: contact, control, speed, discipline</t>
+  </si>
+  <si>
+    <t>utility_hitter</t>
+  </si>
+  <si>
+    <t>Weak Utility</t>
+  </si>
+  <si>
+    <t>Pure Slugger</t>
+  </si>
+  <si>
+    <t>Slugger Only</t>
+  </si>
+  <si>
+    <t>Reliable Contact</t>
+  </si>
+  <si>
+    <t>Omnipresent Contact</t>
   </si>
 </sst>
 </file>
@@ -7786,7 +7801,7 @@
   <dimension ref="A1:Y120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7801,16 +7816,16 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="Y1" t="s">
         <v>17</v>
@@ -7830,12 +7845,12 @@
         <v>2</v>
       </c>
       <c r="Y2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Y3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -7958,7 +7973,7 @@
         <f>IF(B5="",
 IF(B6="",IF(B4="","","    },"),
 CONCATENATE("    ","'",A5,"': {")),
-CONCATENATE("        ","'",B5,"': [",IF(C5="","","'"&amp;C5&amp;"',"),IF(D5="",""," '"&amp;D5&amp;"',"),IF(E5="",""," '"&amp;E5&amp;"',"),IF(F5="",""," '"&amp;F5&amp;"',"),IF(G5="",""," '"&amp;G5&amp;"',"),IF(H5="",""," '"&amp;H5&amp;"',"),IF(I5="",""," '"&amp;I5&amp;"',"),IF(J5="",""," '"&amp;J5&amp;"',"),IF(K5="",""," '"&amp;K5&amp;"',"),IF(L5="",""," '"&amp;L5&amp;"',"),"]"))</f>
+CONCATENATE("        ","'",B5,"': [",IF(C5="","","'"&amp;C5&amp;"',"),IF(D5="",""," '"&amp;D5&amp;"',"),IF(E5="",""," '"&amp;E5&amp;"',"),IF(F5="",""," '"&amp;F5&amp;"',"),IF(G5="",""," '"&amp;G5&amp;"',"),IF(H5="",""," '"&amp;H5&amp;"',"),IF(I5="",""," '"&amp;I5&amp;"',"),IF(J5="",""," '"&amp;J5&amp;"',"),IF(K5="",""," '"&amp;K5&amp;"',"),IF(L5="",""," '"&amp;L5&amp;"',"),"],"))</f>
         <v xml:space="preserve">    'slugging': {</v>
       </c>
     </row>
@@ -7988,10 +8003,10 @@
         <v>slugging</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -8028,8 +8043,8 @@
         <f t="shared" ref="M6:M69" si="2">IF(B6="",
 IF(B7="",IF(B5="","","    },"),
 CONCATENATE("    ","'",A6,"': {")),
-CONCATENATE("        ","'",B6,"': [",IF(C6="","","'"&amp;C6&amp;"',"),IF(D6="",""," '"&amp;D6&amp;"',"),IF(E6="",""," '"&amp;E6&amp;"',"),IF(F6="",""," '"&amp;F6&amp;"',"),IF(G6="",""," '"&amp;G6&amp;"',"),IF(H6="",""," '"&amp;H6&amp;"',"),IF(I6="",""," '"&amp;I6&amp;"',"),IF(J6="",""," '"&amp;J6&amp;"',"),IF(K6="",""," '"&amp;K6&amp;"',"),IF(L6="",""," '"&amp;L6&amp;"',"),"]"))</f>
-        <v xml:space="preserve">        'slugging': ['Weak Slugger', 'Average Slugger', 'Power Slugger',]</v>
+CONCATENATE("        ","'",B6,"': [",IF(C6="","","'"&amp;C6&amp;"',"),IF(D6="",""," '"&amp;D6&amp;"',"),IF(E6="",""," '"&amp;E6&amp;"',"),IF(F6="",""," '"&amp;F6&amp;"',"),IF(G6="",""," '"&amp;G6&amp;"',"),IF(H6="",""," '"&amp;H6&amp;"',"),IF(I6="",""," '"&amp;I6&amp;"',"),IF(J6="",""," '"&amp;J6&amp;"',"),IF(K6="",""," '"&amp;K6&amp;"',"),IF(L6="",""," '"&amp;L6&amp;"',"),"],"))</f>
+        <v xml:space="preserve">        'slugging': ['Slugger Only', 'Pure Slugger', 'Power Slugger',],</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -8096,7 +8111,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Weak Slugger', 'Complete Hitter', 'Complete Clean-Up',]</v>
+        <v xml:space="preserve">        'smallball': ['Weak Slugger', 'Complete Hitter', 'Complete Clean-Up',],</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -8163,7 +8178,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Weak Slugger', 'Average Slugger', 'Fast Power Hitter',]</v>
+        <v xml:space="preserve">        'manufacture': ['Weak Slugger', 'Average Slugger', 'Fast Power Hitter',],</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -8189,18 +8204,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v>slugging: fancy - 0.8</v>
+        <v>slugging: utility_hitter - 0.8</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>slugging: fancy - 2</v>
+        <v>slugging: utility_hitter - 2</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -8232,7 +8247,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Weak Slugger', 'slugging: fancy - 0.8', 'slugging: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Weak Slugger', 'slugging: utility_hitter - 0.8', 'slugging: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -8401,15 +8416,13 @@
         <v>slugging</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="1"/>
-        <v>smallball: slugging - 0.8</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>smallball: slugging - 2</v>
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -8441,7 +8454,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'slugging': ['Weak Contact', 'smallball: slugging - 0.8', 'smallball: slugging - 2',]</v>
+        <v xml:space="preserve">        'slugging': ['Contact Only', 'Reliable Contact', 'Omnipresent Contact',],</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -8470,7 +8483,7 @@
         <v>smallball</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
@@ -8510,7 +8523,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Weak Contact', 'smallball: smallball - 0.8', 'smallball: smallball - 2',]</v>
+        <v xml:space="preserve">        'smallball': ['Weak Contact', 'smallball: smallball - 0.8', 'smallball: smallball - 2',],</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -8539,7 +8552,7 @@
         <v>manufacture</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
@@ -8579,7 +8592,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Weak Contact', 'smallball: manufacture - 0.8', 'smallball: manufacture - 2',]</v>
+        <v xml:space="preserve">        'manufacture': ['Weak Contact', 'smallball: manufacture - 0.8', 'smallball: manufacture - 2',],</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -8605,18 +8618,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>smallball: fancy - 0.8</v>
+        <v>smallball: utility_hitter - 0.8</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>smallball: fancy - 2</v>
+        <v>smallball: utility_hitter - 2</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -8648,7 +8661,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Weak Contact', 'smallball: fancy - 0.8', 'smallball: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Weak Contact', 'smallball: utility_hitter - 0.8', 'smallball: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -8817,7 +8830,7 @@
         <v>slugging</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
@@ -8857,7 +8870,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'slugging': ['Weak Baserunner', 'manufacture: slugging - 0.8', 'manufacture: slugging - 2',]</v>
+        <v xml:space="preserve">        'slugging': ['Weak Baserunner', 'manufacture: slugging - 0.8', 'manufacture: slugging - 2',],</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -8886,7 +8899,7 @@
         <v>smallball</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
@@ -8926,7 +8939,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Weak Baserunner', 'manufacture: smallball - 0.8', 'manufacture: smallball - 2',]</v>
+        <v xml:space="preserve">        'smallball': ['Weak Baserunner', 'manufacture: smallball - 0.8', 'manufacture: smallball - 2',],</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -8955,7 +8968,7 @@
         <v>manufacture</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
@@ -8995,7 +9008,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Weak Baserunner', 'manufacture: manufacture - 0.8', 'manufacture: manufacture - 2',]</v>
+        <v xml:space="preserve">        'manufacture': ['Weak Baserunner', 'manufacture: manufacture - 0.8', 'manufacture: manufacture - 2',],</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -9021,18 +9034,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="3"/>
-        <v>manufacture: fancy - 0.8</v>
+        <v>manufacture: utility_hitter - 0.8</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="3"/>
-        <v>manufacture: fancy - 2</v>
+        <v>manufacture: utility_hitter - 2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="3"/>
@@ -9064,7 +9077,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Weak Baserunner', 'manufacture: fancy - 0.8', 'manufacture: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Weak Baserunner', 'manufacture: utility_hitter - 0.8', 'manufacture: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -9146,7 +9159,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B23" t="str">
         <f>IF(
@@ -9204,7 +9217,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    'fancy': {</v>
+        <v xml:space="preserve">    'utility_hitter': {</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -9216,7 +9229,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B24" t="str">
         <f>IF(
@@ -9233,15 +9246,15 @@
         <v>slugging</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: slugging - 0.8</v>
+        <v>utility_hitter: slugging - 0.8</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: slugging - 2</v>
+        <v>utility_hitter: slugging - 2</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="3"/>
@@ -9273,7 +9286,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'slugging': ['Weak Strategy Hitter', 'fancy: slugging - 0.8', 'fancy: slugging - 2',]</v>
+        <v xml:space="preserve">        'slugging': ['Weak Utility', 'utility_hitter: slugging - 0.8', 'utility_hitter: slugging - 2',],</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -9285,7 +9298,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B25" t="str">
         <f>IF(
@@ -9302,15 +9315,15 @@
         <v>smallball</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: smallball - 0.8</v>
+        <v>utility_hitter: smallball - 0.8</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: smallball - 2</v>
+        <v>utility_hitter: smallball - 2</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="3"/>
@@ -9342,7 +9355,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Weak Strategy Hitter', 'fancy: smallball - 0.8', 'fancy: smallball - 2',]</v>
+        <v xml:space="preserve">        'smallball': ['Weak Utility', 'utility_hitter: smallball - 0.8', 'utility_hitter: smallball - 2',],</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -9354,7 +9367,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B26" t="str">
         <f>IF(
@@ -9371,15 +9384,15 @@
         <v>manufacture</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: manufacture - 0.8</v>
+        <v>utility_hitter: manufacture - 0.8</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: manufacture - 2</v>
+        <v>utility_hitter: manufacture - 2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="3"/>
@@ -9411,7 +9424,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Weak Strategy Hitter', 'fancy: manufacture - 0.8', 'fancy: manufacture - 2',]</v>
+        <v xml:space="preserve">        'manufacture': ['Weak Utility', 'utility_hitter: manufacture - 0.8', 'utility_hitter: manufacture - 2',],</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -9423,7 +9436,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B27" t="str">
         <f>IF(
@@ -9437,18 +9450,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: fancy - 0.8</v>
+        <v>utility_hitter: utility_hitter - 0.8</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
-        <v>fancy: fancy - 2</v>
+        <v>utility_hitter: utility_hitter - 2</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="3"/>
@@ -9480,7 +9493,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Weak Strategy Hitter', 'fancy: fancy - 0.8', 'fancy: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Weak Utility', 'utility_hitter: utility_hitter - 0.8', 'utility_hitter: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -9492,7 +9505,7 @@
         ""),
     INDEX(aspects,1,1+FLOOR((ROW()-ROW(start))/(COUNTA(aspects)+2),1))
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="B28" t="str">
         <f>IF(
@@ -9649,7 +9662,7 @@
         <v>slugging</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="3"/>
@@ -9689,7 +9702,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'slugging': ['Versatile Hitter', 'All: slugging - 0.8', 'All: slugging - 2',]</v>
+        <v xml:space="preserve">        'slugging': ['Versatile Hitter', 'All: slugging - 0.8', 'All: slugging - 2',],</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -9718,7 +9731,7 @@
         <v>smallball</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="3"/>
@@ -9758,7 +9771,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Versatile Hitter', 'All: smallball - 0.8', 'All: smallball - 2',]</v>
+        <v xml:space="preserve">        'smallball': ['Versatile Hitter', 'All: smallball - 0.8', 'All: smallball - 2',],</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -9787,7 +9800,7 @@
         <v>manufacture</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="3"/>
@@ -9827,7 +9840,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Versatile Baserunner', 'All: manufacture - 0.8', 'All: manufacture - 2',]</v>
+        <v xml:space="preserve">        'manufacture': ['Versatile Baserunner', 'All: manufacture - 0.8', 'All: manufacture - 2',],</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -9853,18 +9866,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="3"/>
-        <v>All: fancy - 0.8</v>
+        <v>All: utility_hitter - 0.8</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="3"/>
-        <v>All: fancy - 2</v>
+        <v>All: utility_hitter - 2</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="3"/>
@@ -9896,7 +9909,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Versatile Hitter', 'All: fancy - 0.8', 'All: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Versatile Hitter', 'All: utility_hitter - 0.8', 'All: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -10065,7 +10078,7 @@
         <v>slugging</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="3"/>
@@ -10105,7 +10118,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'slugging': ['Weak Contact', 'Not: slugging - 0.8', 'Not: slugging - 2',]</v>
+        <v xml:space="preserve">        'slugging': ['Weak Contact', 'Not: slugging - 0.8', 'Not: slugging - 2',],</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -10174,7 +10187,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'smallball': ['Weak Slugger', 'Not: smallball - 0.8', 'Not: smallball - 2',]</v>
+        <v xml:space="preserve">        'smallball': ['Weak Slugger', 'Not: smallball - 0.8', 'Not: smallball - 2',],</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -10203,7 +10216,7 @@
         <v>manufacture</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" ref="C38:L69" si="4">IF(OR($B38="", D$4=""),"",CONCATENATE($A38,": ",$B38," - ",D$4))</f>
@@ -10243,7 +10256,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'manufacture': ['Slow Hitter', 'Not: manufacture - 0.8', 'Not: manufacture - 2',]</v>
+        <v xml:space="preserve">        'manufacture': ['Slow Hitter', 'Not: manufacture - 0.8', 'Not: manufacture - 2',],</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -10269,18 +10282,18 @@
             (ROW()-ROW(start)-1),COUNTA(aspects)+2)
     )
 )</f>
-        <v>fancy</v>
+        <v>utility_hitter</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="4"/>
-        <v>Not: fancy - 0.8</v>
+        <v>Not: utility_hitter - 0.8</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="4"/>
-        <v>Not: fancy - 2</v>
+        <v>Not: utility_hitter - 2</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="4"/>
@@ -10312,7 +10325,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">        'fancy': ['Versatile Hitter', 'Not: fancy - 0.8', 'Not: fancy - 2',]</v>
+        <v xml:space="preserve">        'utility_hitter': ['Versatile Hitter', 'Not: utility_hitter - 0.8', 'Not: utility_hitter - 2',],</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -12484,7 +12497,7 @@
         <f t="shared" ref="M70:M120" si="7">IF(B70="",
 IF(B71="",IF(B69="","","    },"),
 CONCATENATE("    ","'",A70,"': {")),
-CONCATENATE("        ","'",B70,"': [",IF(C70="","","'"&amp;C70&amp;"',"),IF(D70="",""," '"&amp;D70&amp;"',"),IF(E70="",""," '"&amp;E70&amp;"',"),IF(F70="",""," '"&amp;F70&amp;"',"),IF(G70="",""," '"&amp;G70&amp;"',"),IF(H70="",""," '"&amp;H70&amp;"',"),IF(I70="",""," '"&amp;I70&amp;"',"),IF(J70="",""," '"&amp;J70&amp;"',"),IF(K70="",""," '"&amp;K70&amp;"',"),IF(L70="",""," '"&amp;L70&amp;"',"),"]"))</f>
+CONCATENATE("        ","'",B70,"': [",IF(C70="","","'"&amp;C70&amp;"',"),IF(D70="",""," '"&amp;D70&amp;"',"),IF(E70="",""," '"&amp;E70&amp;"',"),IF(F70="",""," '"&amp;F70&amp;"',"),IF(G70="",""," '"&amp;G70&amp;"',"),IF(H70="",""," '"&amp;H70&amp;"',"),IF(I70="",""," '"&amp;I70&amp;"',"),IF(J70="",""," '"&amp;J70&amp;"',"),IF(K70="",""," '"&amp;K70&amp;"',"),IF(L70="",""," '"&amp;L70&amp;"',"),"],"))</f>
         <v/>
       </c>
     </row>

</xml_diff>